<commit_message>
Changes made based on Checkstyle report
Roughly 8200 style errors we fixed. Changes and report comparisons can
be found in changes.xlsx, located in the base directory
</commit_message>
<xml_diff>
--- a/changes.xlsx
+++ b/changes.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FindBugs" sheetId="1" r:id="rId1"/>
+    <sheet name="Checkstyle" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +129,30 @@
   </si>
   <si>
     <t>After</t>
+  </si>
+  <si>
+    <t>Checkstyle</t>
+  </si>
+  <si>
+    <t>Javadocs generated to reduce instances of missing Javadoc comments</t>
+  </si>
+  <si>
+    <t>Unit.java</t>
+  </si>
+  <si>
+    <t>src directory</t>
+  </si>
+  <si>
+    <t>Removed redundant import statements</t>
+  </si>
+  <si>
+    <t>Added braces to various 'if' constructs where they were missing</t>
+  </si>
+  <si>
+    <t>Player.java</t>
+  </si>
+  <si>
+    <t>Source&gt;Format removed many spacing errors</t>
   </si>
 </sst>
 </file>
@@ -171,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -185,6 +210,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -285,6 +316,94 @@
         <a:xfrm>
           <a:off x="7019925" y="13163550"/>
           <a:ext cx="5800725" cy="2905703"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="18104762" cy="1571429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DECF4DC3-4FE5-49CE-B674-DBCF0ED57890}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3248025"/>
+          <a:ext cx="18104762" cy="1571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>35836</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>66481</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32A4D4A2-16A8-427A-BD32-EA8836D4235D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5734050"/>
+          <a:ext cx="18114286" cy="1552381"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -559,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F48"/>
+  <dimension ref="A2:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,55 +941,260 @@
     <row r="32" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="3"/>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="69.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>42870</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>42870</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>42870</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>42870</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>42870</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>42870</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>